<commit_message>
update gold tables without duplicated data
</commit_message>
<xml_diff>
--- a/data/tables_gold/gold.sih_2024_icsap_category.xlsx
+++ b/data/tables_gold/gold.sih_2024_icsap_category.xlsx
@@ -471,20 +471,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Infecção no Rim e Trato Urinário</t>
+          <t>Hipertensão</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>218241</v>
+        <v>37068</v>
       </c>
       <c r="D2" t="n">
-        <v>126877175.19</v>
+        <v>18044255.16</v>
       </c>
       <c r="E2" t="n">
-        <v>581.36</v>
+        <v>486.79</v>
       </c>
       <c r="F2" t="n">
-        <v>5.67</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="3">
@@ -493,20 +493,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Doencas pulmonares</t>
+          <t>Doenças preveníveis por imunização e condições sensíveis</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>18493</v>
+        <v>17733</v>
       </c>
       <c r="D3" t="n">
-        <v>12387346.96</v>
+        <v>26005097.38</v>
       </c>
       <c r="E3" t="n">
-        <v>669.84</v>
+        <v>1466.48</v>
       </c>
       <c r="F3" t="n">
-        <v>4.09</v>
+        <v>15.83</v>
       </c>
     </row>
     <row r="4">
@@ -515,20 +515,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Infecção da pele e tecido subcutâneo</t>
+          <t>Doenças relacionadas ao Pré-Natal e Parto</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>41557</v>
+        <v>168</v>
       </c>
       <c r="D4" t="n">
-        <v>26165231.64</v>
+        <v>261426.06</v>
       </c>
       <c r="E4" t="n">
-        <v>629.62</v>
+        <v>1556.11</v>
       </c>
       <c r="F4" t="n">
-        <v>6.52</v>
+        <v>8.34</v>
       </c>
     </row>
     <row r="5">
@@ -537,20 +537,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Doença Inflamatória órgãos pélvicos femininos</t>
+          <t>Diabetes melitus</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1081</v>
+        <v>136172</v>
       </c>
       <c r="D5" t="n">
-        <v>480510.46</v>
+        <v>151124585.96</v>
       </c>
       <c r="E5" t="n">
-        <v>444.51</v>
+        <v>1109.81</v>
       </c>
       <c r="F5" t="n">
-        <v>2.45</v>
+        <v>6.78</v>
       </c>
     </row>
     <row r="6">
@@ -559,42 +559,42 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Asma</t>
+          <t>Úlcera gastrointestinal</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6492</v>
+        <v>50844</v>
       </c>
       <c r="D6" t="n">
-        <v>4849799.21</v>
+        <v>60521054.37</v>
       </c>
       <c r="E6" t="n">
-        <v>747.04</v>
+        <v>1190.33</v>
       </c>
       <c r="F6" t="n">
-        <v>3.43</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2014</v>
+        <v>2024</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Doenças preveníveis por imunização e condições sensíveis</t>
+          <t>Pneumonias bacterianas</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17743</v>
+        <v>168655</v>
       </c>
       <c r="D7" t="n">
-        <v>26030165.22</v>
+        <v>243172884.92</v>
       </c>
       <c r="E7" t="n">
-        <v>1467.07</v>
+        <v>1441.84</v>
       </c>
       <c r="F7" t="n">
-        <v>15.84</v>
+        <v>6.83</v>
       </c>
     </row>
     <row r="8">
@@ -603,20 +603,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Doenças relacionadas ao Pré-Natal e Parto</t>
+          <t>Doenças Cerebrovasculares</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>168</v>
+        <v>141909</v>
       </c>
       <c r="D8" t="n">
-        <v>261426.06</v>
+        <v>172055725.92</v>
       </c>
       <c r="E8" t="n">
-        <v>1556.11</v>
+        <v>1212.44</v>
       </c>
       <c r="F8" t="n">
-        <v>8.34</v>
+        <v>7.72</v>
       </c>
     </row>
     <row r="9">
@@ -625,20 +625,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hipertensão</t>
+          <t>Doenças Cerebrovasculares</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>37069</v>
+        <v>197963</v>
       </c>
       <c r="D9" t="n">
-        <v>18047013.21</v>
+        <v>365759200.23</v>
       </c>
       <c r="E9" t="n">
-        <v>486.85</v>
+        <v>1847.61</v>
       </c>
       <c r="F9" t="n">
-        <v>4.22</v>
+        <v>7.29</v>
       </c>
     </row>
     <row r="10">
@@ -647,20 +647,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gastroenterites Infecciosas e complicações</t>
+          <t>Diabetes melitus</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>204186</v>
+        <v>139819</v>
       </c>
       <c r="D10" t="n">
-        <v>67409507.34999999</v>
+        <v>89667747.68000001</v>
       </c>
       <c r="E10" t="n">
-        <v>330.14</v>
+        <v>641.3099999999999</v>
       </c>
       <c r="F10" t="n">
-        <v>3.11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -669,64 +669,64 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Deficiências Nutricionais</t>
+          <t>Pneumonias bacterianas</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>37174</v>
+        <v>149040</v>
       </c>
       <c r="D11" t="n">
-        <v>24500807.12</v>
+        <v>152952601.45</v>
       </c>
       <c r="E11" t="n">
-        <v>659.08</v>
+        <v>1026.25</v>
       </c>
       <c r="F11" t="n">
-        <v>7.25</v>
+        <v>6.27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2024</v>
+        <v>2014</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Insuficiência Cardíaca</t>
+          <t>Úlcera gastrointestinal</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>26020</v>
+        <v>26980</v>
       </c>
       <c r="D12" t="n">
-        <v>71171979.81</v>
+        <v>20666487.39</v>
       </c>
       <c r="E12" t="n">
-        <v>2735.28</v>
+        <v>765.99</v>
       </c>
       <c r="F12" t="n">
-        <v>8.26</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2014</v>
+        <v>2024</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Doença Inflamatória órgãos pélvicos femininos</t>
+          <t>Infecções de ouvido, nariz e garganta</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>309</v>
+        <v>2239</v>
       </c>
       <c r="D13" t="n">
-        <v>72067.13</v>
+        <v>670022.02</v>
       </c>
       <c r="E13" t="n">
-        <v>233.23</v>
+        <v>299.25</v>
       </c>
       <c r="F13" t="n">
-        <v>1.7</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="14">
@@ -735,20 +735,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Asma</t>
+          <t>Infecção no Rim e Trato Urinário</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>12292</v>
+        <v>186646</v>
       </c>
       <c r="D14" t="n">
-        <v>6598149.13</v>
+        <v>63451630.38</v>
       </c>
       <c r="E14" t="n">
-        <v>536.78</v>
+        <v>339.96</v>
       </c>
       <c r="F14" t="n">
-        <v>2.93</v>
+        <v>4.47</v>
       </c>
     </row>
     <row r="15">
@@ -801,20 +801,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Pneumonias bacterianas</t>
+          <t>Asma</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>149040</v>
+        <v>12292</v>
       </c>
       <c r="D17" t="n">
-        <v>152952601.45</v>
+        <v>6598149.13</v>
       </c>
       <c r="E17" t="n">
-        <v>1026.25</v>
+        <v>536.78</v>
       </c>
       <c r="F17" t="n">
-        <v>6.27</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="18">
@@ -823,64 +823,64 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Diabetes melitus</t>
+          <t>Doença Inflamatória órgãos pélvicos femininos</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>139819</v>
+        <v>309</v>
       </c>
       <c r="D18" t="n">
-        <v>89667747.68000001</v>
+        <v>72067.13</v>
       </c>
       <c r="E18" t="n">
-        <v>641.3099999999999</v>
+        <v>233.23</v>
       </c>
       <c r="F18" t="n">
-        <v>6</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2014</v>
+        <v>2024</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Úlcera gastrointestinal</t>
+          <t>Insuficiência Cardíaca</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>26980</v>
+        <v>26020</v>
       </c>
       <c r="D19" t="n">
-        <v>20666487.39</v>
+        <v>71171979.81</v>
       </c>
       <c r="E19" t="n">
-        <v>765.99</v>
+        <v>2735.28</v>
       </c>
       <c r="F19" t="n">
-        <v>5.38</v>
+        <v>8.26</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2024</v>
+        <v>2014</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Doenças Cerebrovasculares</t>
+          <t>Gastroenterites Infecciosas e complicações</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>197963</v>
+        <v>204186</v>
       </c>
       <c r="D20" t="n">
-        <v>365759200.23</v>
+        <v>67409507.34999999</v>
       </c>
       <c r="E20" t="n">
-        <v>1847.61</v>
+        <v>330.14</v>
       </c>
       <c r="F20" t="n">
-        <v>7.29</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="21">
@@ -889,20 +889,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Doenças Cerebrovasculares</t>
+          <t>Deficiências Nutricionais</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>141909</v>
+        <v>37174</v>
       </c>
       <c r="D21" t="n">
-        <v>172055725.92</v>
+        <v>24500807.12</v>
       </c>
       <c r="E21" t="n">
-        <v>1212.44</v>
+        <v>659.08</v>
       </c>
       <c r="F21" t="n">
-        <v>7.72</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="22">
@@ -911,20 +911,20 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Úlcera gastrointestinal</t>
+          <t>Infecção no Rim e Trato Urinário</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>50844</v>
+        <v>218241</v>
       </c>
       <c r="D22" t="n">
-        <v>60521054.37</v>
+        <v>126877175.19</v>
       </c>
       <c r="E22" t="n">
-        <v>1190.33</v>
+        <v>581.36</v>
       </c>
       <c r="F22" t="n">
-        <v>5.6</v>
+        <v>5.67</v>
       </c>
     </row>
     <row r="23">
@@ -933,20 +933,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Pneumonias bacterianas</t>
+          <t>Gastroenterites Infecciosas e complicações</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>168655</v>
+        <v>126223</v>
       </c>
       <c r="D23" t="n">
-        <v>243172884.92</v>
+        <v>51377873.76</v>
       </c>
       <c r="E23" t="n">
-        <v>1441.84</v>
+        <v>407.04</v>
       </c>
       <c r="F23" t="n">
-        <v>6.83</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="24">
@@ -955,64 +955,64 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Diabetes melitus</t>
+          <t>Deficiências Nutricionais</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>136172</v>
+        <v>19316</v>
       </c>
       <c r="D24" t="n">
-        <v>151124585.96</v>
+        <v>24227126.98</v>
       </c>
       <c r="E24" t="n">
-        <v>1109.81</v>
+        <v>1254.25</v>
       </c>
       <c r="F24" t="n">
-        <v>6.78</v>
+        <v>8.67</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2024</v>
+        <v>2014</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Infecções de ouvido, nariz e garganta</t>
+          <t>Insuficiência Cardíaca</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2239</v>
+        <v>13725</v>
       </c>
       <c r="D25" t="n">
-        <v>670022.02</v>
+        <v>24408951.27</v>
       </c>
       <c r="E25" t="n">
-        <v>299.25</v>
+        <v>1778.43</v>
       </c>
       <c r="F25" t="n">
-        <v>2.89</v>
+        <v>7.02</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2014</v>
+        <v>2024</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Infecções de ouvido, nariz e garganta</t>
+          <t>Eplepsias</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>84</v>
+        <v>1485</v>
       </c>
       <c r="D26" t="n">
-        <v>5391.6</v>
+        <v>1473095.85</v>
       </c>
       <c r="E26" t="n">
-        <v>64.19</v>
+        <v>991.98</v>
       </c>
       <c r="F26" t="n">
-        <v>1.52</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="27">
@@ -1021,20 +1021,20 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Angina</t>
+          <t>Doenças preveníveis por imunização e condições sensíveis</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1132</v>
+        <v>23839</v>
       </c>
       <c r="D27" t="n">
-        <v>5301099.39</v>
+        <v>46300850.19</v>
       </c>
       <c r="E27" t="n">
-        <v>4682.95</v>
+        <v>1942.23</v>
       </c>
       <c r="F27" t="n">
-        <v>4.87</v>
+        <v>13.73</v>
       </c>
     </row>
     <row r="28">
@@ -1043,20 +1043,20 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Insuficiência Cardíaca</t>
+          <t>Hipertensão</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>13725</v>
+        <v>77945</v>
       </c>
       <c r="D28" t="n">
-        <v>24408951.27</v>
+        <v>26713533.69</v>
       </c>
       <c r="E28" t="n">
-        <v>1778.43</v>
+        <v>342.72</v>
       </c>
       <c r="F28" t="n">
-        <v>7.02</v>
+        <v>4.34</v>
       </c>
     </row>
     <row r="29">
@@ -1065,20 +1065,20 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Gastroenterites Infecciosas e complicações</t>
+          <t>Anemia</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>126223</v>
+        <v>1121</v>
       </c>
       <c r="D29" t="n">
-        <v>51377873.76</v>
+        <v>446850.07</v>
       </c>
       <c r="E29" t="n">
-        <v>407.04</v>
+        <v>398.62</v>
       </c>
       <c r="F29" t="n">
-        <v>3.33</v>
+        <v>3.99</v>
       </c>
     </row>
     <row r="30">
@@ -1087,20 +1087,20 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Deficiências Nutricionais</t>
+          <t>Doenças relacionadas ao Pré-Natal e Parto</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>19316</v>
+        <v>1827</v>
       </c>
       <c r="D30" t="n">
-        <v>24227126.98</v>
+        <v>1143375.44</v>
       </c>
       <c r="E30" t="n">
-        <v>1254.25</v>
+        <v>625.8200000000001</v>
       </c>
       <c r="F30" t="n">
-        <v>8.67</v>
+        <v>6.28</v>
       </c>
     </row>
     <row r="31">
@@ -1109,20 +1109,20 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Eplepsias</t>
+          <t>Asma</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1485</v>
+        <v>6492</v>
       </c>
       <c r="D31" t="n">
-        <v>1473095.85</v>
+        <v>4849799.21</v>
       </c>
       <c r="E31" t="n">
-        <v>991.98</v>
+        <v>747.04</v>
       </c>
       <c r="F31" t="n">
-        <v>5.62</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="32">
@@ -1131,42 +1131,42 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Hipertensão</t>
+          <t>Doencas pulmonares</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>77948</v>
+        <v>18493</v>
       </c>
       <c r="D32" t="n">
-        <v>26720485.44</v>
+        <v>12387346.96</v>
       </c>
       <c r="E32" t="n">
-        <v>342.8</v>
+        <v>669.84</v>
       </c>
       <c r="F32" t="n">
-        <v>4.34</v>
+        <v>4.09</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2024</v>
+        <v>2014</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Doenças preveníveis por imunização e condições sensíveis</t>
+          <t>Infecção da pele e tecido subcutâneo</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>23845</v>
+        <v>41557</v>
       </c>
       <c r="D33" t="n">
-        <v>46316432.11</v>
+        <v>26165231.64</v>
       </c>
       <c r="E33" t="n">
-        <v>1942.4</v>
+        <v>629.62</v>
       </c>
       <c r="F33" t="n">
-        <v>13.73</v>
+        <v>6.52</v>
       </c>
     </row>
     <row r="34">
@@ -1175,20 +1175,20 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Doenças relacionadas ao Pré-Natal e Parto</t>
+          <t>Doença Inflamatória órgãos pélvicos femininos</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1827</v>
+        <v>1081</v>
       </c>
       <c r="D34" t="n">
-        <v>1143375.44</v>
+        <v>480510.46</v>
       </c>
       <c r="E34" t="n">
-        <v>625.8200000000001</v>
+        <v>444.51</v>
       </c>
       <c r="F34" t="n">
-        <v>6.28</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="35">
@@ -1197,20 +1197,20 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Anemia</t>
+          <t>Angina</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1121</v>
+        <v>1132</v>
       </c>
       <c r="D35" t="n">
-        <v>446850.07</v>
+        <v>5301099.39</v>
       </c>
       <c r="E35" t="n">
-        <v>398.62</v>
+        <v>4682.95</v>
       </c>
       <c r="F35" t="n">
-        <v>3.99</v>
+        <v>4.87</v>
       </c>
     </row>
     <row r="36">
@@ -1219,20 +1219,20 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Infecção no Rim e Trato Urinário</t>
+          <t>Infecções de ouvido, nariz e garganta</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>186646</v>
+        <v>84</v>
       </c>
       <c r="D36" t="n">
-        <v>63451630.38</v>
+        <v>5391.6</v>
       </c>
       <c r="E36" t="n">
-        <v>339.96</v>
+        <v>64.19</v>
       </c>
       <c r="F36" t="n">
-        <v>4.47</v>
+        <v>1.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>